<commit_message>
First day data science
</commit_message>
<xml_diff>
--- a/Presentations/Data Science/Linear Regression.xlsx
+++ b/Presentations/Data Science/Linear Regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\OneDrive\Documentos\Utilidades\Unison\006 CSI\JGCC Python Course\Presentations\Data Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A880C4-74B5-4252-AE29-3E2A19D86E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5DE37A-3EA2-4829-9729-30F01E4EC1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1607,7 +1607,7 @@
   <dimension ref="C2:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+      <selection activeCell="F3" sqref="F3:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>